<commit_message>
Adding different messages to the InputException for different input types
</commit_message>
<xml_diff>
--- a/Enrollment_Log.xlsx
+++ b/Enrollment_Log.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Subject_ID</t>
   </si>
@@ -74,6 +74,27 @@
   </si>
   <si>
     <t>13:11:37.430766</t>
+  </si>
+  <si>
+    <t>22:01:36.640593</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>-0</t>
+  </si>
+  <si>
+    <t>22:03:54.603169</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -439,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C8" activeCellId="0" pane="topLeft" sqref="C8"/>
@@ -615,6 +636,52 @@
       </c>
       <c r="G7" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>